<commit_message>
this is my new change
</commit_message>
<xml_diff>
--- a/copy of list.xlsx
+++ b/copy of list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>NAME OF ENETRPRISE</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>https://gruhudyog.in/  LINK TO SEE ALL</t>
+  </si>
+  <si>
+    <t>to avail all details</t>
   </si>
 </sst>
 </file>
@@ -577,7 +580,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,6 +782,9 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>